<commit_message>
presentation add raw erd diagram gen by DBeaver
</commit_message>
<xml_diff>
--- a/presentation/partyCommFuncServiceData.xlsx
+++ b/presentation/partyCommFuncServiceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scwork\year4_final\proj\crud_from_datamodel\party_fullstack_docker3\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4EFCA7-DF3F-4590-9651-1C1BB7982069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC64A319-7760-4F12-96E7-44616275F92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37EAAD1-7031-40FC-AF7B-2DF2BDACF713}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5348351A-2786-4AA3-BFCD-3E5CC451ECFA}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8E9532-D2C7-46E6-9732-064C995064AA}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
backend layertype for role relation commu fin but not test
</commit_message>
<xml_diff>
--- a/presentation/partyCommFuncServiceData.xlsx
+++ b/presentation/partyCommFuncServiceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scwork\year4_final\proj\crud_from_datamodel\party_fullstack_docker3\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC64A319-7760-4F12-96E7-44616275F92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D039DFA7-2836-4234-AF18-84A8E9B9A959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37EAAD1-7031-40FC-AF7B-2DF2BDACF713}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -858,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5348351A-2786-4AA3-BFCD-3E5CC451ECFA}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>